<commit_message>
added Availability sets , VM and Storage
</commit_message>
<xml_diff>
--- a/Igloo-srv-list.xlsx
+++ b/Igloo-srv-list.xlsx
@@ -30,15 +30,6 @@
     <t>Server</t>
   </si>
   <si>
-    <t>Operating System</t>
-  </si>
-  <si>
-    <t>OS Disk in GBs (VMWare)</t>
-  </si>
-  <si>
-    <t>Data Disk in GBs (VMWware)</t>
-  </si>
-  <si>
     <t>Azure Instance Type</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
     <t>Windows Update Services (WSUS)</t>
   </si>
   <si>
-    <t>Server Name</t>
-  </si>
-  <si>
     <t>POC-EUS-Deploy-Linux</t>
   </si>
   <si>
@@ -375,9 +363,6 @@
     <t>POC-EUS-WSUS</t>
   </si>
   <si>
-    <t>Name Length</t>
-  </si>
-  <si>
     <t>A2v2</t>
   </si>
   <si>
@@ -402,9 +387,6 @@
     <t>ImageName</t>
   </si>
   <si>
-    <t>Storage Account</t>
-  </si>
-  <si>
     <t>CentOS73</t>
   </si>
   <si>
@@ -474,9 +456,6 @@
     <t>mgmt</t>
   </si>
   <si>
-    <t>Availability Set</t>
-  </si>
-  <si>
     <t>Igloo-POC-Web-AS</t>
   </si>
   <si>
@@ -792,9 +771,6 @@
     <t>Standard_M128s</t>
   </si>
   <si>
-    <t>VM Size Code</t>
-  </si>
-  <si>
     <t>Win2012R2</t>
   </si>
   <si>
@@ -802,6 +778,30 @@
   </si>
   <si>
     <t>igloovmstorageprem</t>
+  </si>
+  <si>
+    <t>ServerName</t>
+  </si>
+  <si>
+    <t>NameLength</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>StorageAccount</t>
+  </si>
+  <si>
+    <t>AvailabilitySet</t>
+  </si>
+  <si>
+    <t>OSDiskSize</t>
+  </si>
+  <si>
+    <t>DataDiskSize</t>
+  </si>
+  <si>
+    <t>VMSize</t>
   </si>
 </sst>
 </file>
@@ -958,19 +958,19 @@
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" name="Server" dataDxfId="11"/>
-    <tableColumn id="6" name="Server Name" dataDxfId="10"/>
-    <tableColumn id="7" name="Name Length" dataDxfId="9">
-      <calculatedColumnFormula>LEN(Table1[[#This Row],[Server Name]])</calculatedColumnFormula>
+    <tableColumn id="6" name="ServerName" dataDxfId="10"/>
+    <tableColumn id="7" name="NameLength" dataDxfId="9">
+      <calculatedColumnFormula>LEN(Table1[[#This Row],[ServerName]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Operating System" dataDxfId="8"/>
-    <tableColumn id="9" name="ImageName" dataDxfId="3"/>
-    <tableColumn id="10" name="Storage Account" dataDxfId="2"/>
-    <tableColumn id="8" name="subnet" dataDxfId="7"/>
-    <tableColumn id="11" name="Availability Set" dataDxfId="1"/>
-    <tableColumn id="3" name="OS Disk in GBs (VMWare)" dataDxfId="6"/>
-    <tableColumn id="4" name="Data Disk in GBs (VMWware)" dataDxfId="5"/>
-    <tableColumn id="5" name="Azure Instance Type" dataDxfId="4"/>
-    <tableColumn id="12" name="VM Size Code" dataDxfId="0"/>
+    <tableColumn id="2" name="OS" dataDxfId="8"/>
+    <tableColumn id="9" name="ImageName" dataDxfId="7"/>
+    <tableColumn id="10" name="StorageAccount" dataDxfId="6"/>
+    <tableColumn id="8" name="subnet" dataDxfId="5"/>
+    <tableColumn id="11" name="AvailabilitySet" dataDxfId="4"/>
+    <tableColumn id="3" name="OSDiskSize" dataDxfId="3"/>
+    <tableColumn id="4" name="DataDiskSize" dataDxfId="2"/>
+    <tableColumn id="5" name="Azure Instance Type" dataDxfId="1"/>
+    <tableColumn id="12" name="VMSize" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1290,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1310,103 +1310,103 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>251</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>252</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C2" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I2" s="3">
         <v>20</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I3" s="3">
         <v>20</v>
@@ -1415,37 +1415,37 @@
         <v>80</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C4" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I4" s="3">
         <v>20</v>
@@ -1454,37 +1454,37 @@
         <v>80</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C5" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I5" s="3">
         <v>20</v>
@@ -1493,37 +1493,37 @@
         <v>80</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C6" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I6" s="3">
         <v>20</v>
@@ -1532,37 +1532,37 @@
         <v>50</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C7" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I7" s="3">
         <v>20</v>
@@ -1571,37 +1571,37 @@
         <v>50</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C8" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I8" s="3">
         <v>20</v>
@@ -1610,37 +1610,37 @@
         <v>50</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C9" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I9" s="3">
         <v>16</v>
@@ -1649,37 +1649,37 @@
         <v>80</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C10" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I10" s="3">
         <v>16</v>
@@ -1688,37 +1688,37 @@
         <v>80</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C11" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I11" s="3">
         <v>16</v>
@@ -1727,37 +1727,37 @@
         <v>80</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C12" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I12" s="3">
         <v>20</v>
@@ -1766,466 +1766,466 @@
         <v>50</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C13" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I13" s="3">
         <v>20</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C14" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>14</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I14" s="3">
         <v>40</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C15" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="G15" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I15" s="3">
         <v>40</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C16" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I16" s="3">
         <v>40</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C17" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>14</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="H17" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I17" s="3">
         <v>40</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C18" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I18" s="3">
         <v>20</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C19" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I19" s="3">
         <v>20</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C20" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I20" s="3">
         <v>20</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C21" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>12</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I21" s="3">
         <v>40</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C22" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>12</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I22" s="3">
         <v>40</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C23" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>10</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I23" s="3">
         <v>40</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C24" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>11</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I24" s="3">
         <v>40</v>
@@ -2234,505 +2234,505 @@
         <v>300</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C25" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>12</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I25" s="3">
         <v>60</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C26" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>14</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I26" s="3">
         <v>60</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C27" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>14</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I27" s="3">
         <v>60</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C28" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I28" s="3">
         <v>40</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C29" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I29" s="3">
         <v>40</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C30" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>12</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I30" s="3">
         <v>60</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C31" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I31" s="3">
         <v>60</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C32" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I32" s="3">
         <v>60</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C33" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>15</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I33" s="3">
         <v>40</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C34" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>15</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I34" s="3">
         <v>40</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C35" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I35" s="3">
         <v>40</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C36" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I36" s="3">
         <v>40</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C37" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I37" s="3">
         <v>40</v>
@@ -2741,583 +2741,583 @@
         <v>15</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C38" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I38" s="3">
         <v>400</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C39" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>15</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I39" s="3">
         <v>40</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C40" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>15</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I40" s="3">
         <v>40</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C41" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I41" s="3">
         <v>40</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C42" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I42" s="3">
         <v>40</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C43" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>11</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I43" s="3">
         <v>60</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C44" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>12</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I44" s="3">
         <v>135</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C45" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>15</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I45" s="3">
         <v>90</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C46" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I46" s="3">
         <v>60</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C47" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I47" s="3">
         <v>60</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C48" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I48" s="3">
         <v>60</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C49" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I49" s="3">
         <v>60</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C50" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I50" s="3">
         <v>60</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C51" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="I51" s="3">
         <v>60</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C52" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>12</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I52" s="3">
         <v>60</v>
@@ -3326,115 +3326,115 @@
         <v>200</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C53" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I53" s="3">
         <v>60</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C54" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I54" s="3">
         <v>60</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C55" s="4">
-        <f>LEN(Table1[[#This Row],[Server Name]])</f>
+        <f>LEN(Table1[[#This Row],[ServerName]])</f>
         <v>13</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I55" s="3">
         <v>40</v>
@@ -3443,10 +3443,10 @@
         <v>2048</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3490,27 +3490,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3530,7 +3530,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3550,7 +3550,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3570,7 +3570,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -3630,7 +3630,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -3650,7 +3650,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -3670,7 +3670,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3690,7 +3690,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3710,7 +3710,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3730,7 +3730,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3750,7 +3750,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -3770,7 +3770,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -3810,7 +3810,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -3830,7 +3830,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B19">
         <v>16</v>
@@ -3870,7 +3870,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -3890,7 +3890,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -3910,7 +3910,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -3930,7 +3930,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B23">
         <v>16</v>
@@ -3950,7 +3950,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B24">
         <v>20</v>
@@ -3970,7 +3970,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -4010,7 +4010,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -4030,7 +4030,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B28">
         <v>16</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -4070,7 +4070,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B30">
         <v>4</v>
@@ -4090,7 +4090,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -4110,7 +4110,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B32">
         <v>16</v>
@@ -4130,7 +4130,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -4150,7 +4150,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B35">
         <v>4</v>
@@ -4190,7 +4190,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B37">
         <v>16</v>
@@ -4230,7 +4230,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -4250,7 +4250,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -4270,7 +4270,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -4330,7 +4330,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -4350,7 +4350,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B44">
         <v>8</v>
@@ -4370,7 +4370,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4390,7 +4390,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -4410,7 +4410,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -4430,7 +4430,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B48">
         <v>8</v>
@@ -4450,7 +4450,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B49">
         <v>16</v>
@@ -4470,7 +4470,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -4510,7 +4510,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B52">
         <v>8</v>
@@ -4530,7 +4530,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B53">
         <v>16</v>
@@ -4550,7 +4550,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B54">
         <v>20</v>
@@ -4570,7 +4570,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -4590,7 +4590,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -4610,7 +4610,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4630,7 +4630,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B58">
         <v>16</v>
@@ -4650,7 +4650,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -4670,7 +4670,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B60">
         <v>4</v>
@@ -4690,7 +4690,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -4710,7 +4710,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B62">
         <v>16</v>
@@ -4730,7 +4730,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -4750,7 +4750,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B64">
         <v>2</v>
@@ -4770,7 +4770,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B65">
         <v>4</v>
@@ -4790,7 +4790,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B67">
         <v>16</v>
@@ -4830,7 +4830,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -4850,7 +4850,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B69">
         <v>2</v>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4890,7 +4890,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4910,7 +4910,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -4930,7 +4930,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B73">
         <v>4</v>
@@ -4950,7 +4950,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4970,7 +4970,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B75">
         <v>16</v>
@@ -4990,7 +4990,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -5010,7 +5010,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B77">
         <v>4</v>
@@ -5030,7 +5030,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B78">
         <v>8</v>
@@ -5050,7 +5050,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -5070,7 +5070,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B80">
         <v>32</v>
@@ -5090,7 +5090,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -5110,7 +5110,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -5130,7 +5130,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -5150,7 +5150,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B84">
         <v>16</v>
@@ -5170,7 +5170,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B85">
         <v>32</v>
@@ -5190,7 +5190,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B86">
         <v>4</v>
@@ -5210,7 +5210,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B87">
         <v>8</v>
@@ -5230,7 +5230,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B88">
         <v>16</v>
@@ -5250,7 +5250,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B89">
         <v>32</v>
@@ -5270,7 +5270,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -5290,7 +5290,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -5310,7 +5310,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B92">
         <v>4</v>
@@ -5330,7 +5330,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B93">
         <v>8</v>
@@ -5350,7 +5350,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -5370,7 +5370,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -5390,7 +5390,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B96">
         <v>8</v>
@@ -5410,7 +5410,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B97">
         <v>16</v>
@@ -5430,7 +5430,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B98">
         <v>64</v>
@@ -5450,7 +5450,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B99">
         <v>128</v>

</xml_diff>